<commit_message>
Aero update; Solver update; Degenerate mass problem solved
</commit_message>
<xml_diff>
--- a/Aero/Ansys/Aero2.xlsx
+++ b/Aero/Ansys/Aero2.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescovalentia/ULB/MA1/Formula student/Github2.0/Aero/Ansys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F75CB4-C379-1949-9377-E19E8C117AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87AB74A-8EFE-CB48-BE16-734EAB6A5CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{13B2791B-E7CF-8847-9FFD-1B79316A0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$2:$D$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$F$2:$F$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,9 +45,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>speed</t>
-  </si>
-  <si>
     <t>Lift_reduced</t>
   </si>
   <si>
@@ -51,6 +55,9 @@
   </si>
   <si>
     <t>Drag[N]</t>
+  </si>
+  <si>
+    <t>speed[m/s]</t>
   </si>
 </sst>
 </file>
@@ -111,6 +118,1197 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-19.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-76.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CCB9-D745-98BF-6ECC47726F24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-CCB9-D745-98BF-6ECC47726F24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1960319936"/>
+        <c:axId val="1960339088"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.76800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.76890000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.78749999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CCB9-D745-98BF-6ECC47726F24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.84799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-CCB9-D745-98BF-6ECC47726F24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="376565600"/>
+        <c:axId val="376459280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1960319936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1960339088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1960339088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1960319936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="376459280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="376565600"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="376565600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="376459280"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>195385</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693615</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>37123</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CC37EFC-643C-FEA4-461D-C7E314C9A5F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,106 +1628,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C17050-C296-6448-A912-C3AA3D2684BE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>-19.2</v>
+      </c>
+      <c r="D2">
+        <f>C2/(B2^2)</f>
+        <v>-0.76800000000000002</v>
+      </c>
+      <c r="E2">
+        <v>21.2</v>
+      </c>
+      <c r="F2">
+        <f>E2/(B2^2)</f>
+        <v>0.84799999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>-76.89</v>
       </c>
-      <c r="C2">
-        <f>B2/(A2^2)</f>
+      <c r="D3">
+        <f>C3/(B3^2)</f>
         <v>-0.76890000000000003</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>82.8</v>
       </c>
-      <c r="E2">
-        <f>D2/(A2^2)</f>
+      <c r="F3">
+        <f>E3/(B3^2)</f>
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>-315</v>
       </c>
-      <c r="C3">
-        <f>B3/(A3^2)</f>
+      <c r="D4">
+        <f>C4/(B4^2)</f>
         <v>-0.78749999999999998</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>334</v>
       </c>
-      <c r="E3">
-        <f>D3/(A3^2)</f>
+      <c r="F4">
+        <f>E4/(B4^2)</f>
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>-19.2</v>
-      </c>
-      <c r="C4">
-        <f>B4/(A4^2)</f>
-        <v>-0.76800000000000002</v>
-      </c>
-      <c r="D4">
-        <v>21.2</v>
-      </c>
-      <c r="E4">
-        <f>D4/(A4^2)</f>
-        <v>0.84799999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6">
-        <f>AVERAGE(C2:C4)</f>
-        <v>-0.77479999999999993</v>
-      </c>
-      <c r="E6">
-        <f>AVERAGE(E2:E4)</f>
-        <v>0.83699999999999986</v>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f>AVERAGE(D3:D4)</f>
+        <v>-0.7782</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(F3:F4)</f>
+        <v>0.83149999999999991</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>